<commit_message>
Se crea el metodo testAlertTextError para hacer las validaciones de que genere mensaje de error para cada ingreso erroneo de los campos
</commit_message>
<xml_diff>
--- a/Diseño de pruebas.xlsx
+++ b/Diseño de pruebas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sofka\curso\6. Automatizacion\RetoAutomatizacionConSelenium\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sofka\curso\6. Automatizacion\Reto1\AutomatizacionSelenium\RetoAutoSelenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEACD21-D3F6-4595-9E8F-E63D3972F184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7757298-10D4-4A13-9CAC-68A56F892E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="4320" windowWidth="20400" windowHeight="6945" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consolidado" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="75">
   <si>
     <t>Módulo</t>
   </si>
@@ -252,8 +252,40 @@
 2, Verificar que cargue una nueva página con campos para enviar mensaje a la compañía</t>
   </si>
   <si>
-    <t xml:space="preserve">1, Hacer clic en el botón "Contact us"
-2, </t>
+    <t>1, Hacer clic en el botón "Contact us"
+2, Verificar que aparezcan los elementos , (Subject Heading, Email address, Order reference, Attach File, Message).</t>
+  </si>
+  <si>
+    <t>Debe aparecer error si no se selecciona Subject Heading.</t>
+  </si>
+  <si>
+    <t>Al llenar todos los elementos y enviar el mensaje, debe aparecer un mensaje de confirmación del envió.</t>
+  </si>
+  <si>
+    <t>1, Hacer clic en el botón "Contact us"
+2, llenar todos los campos de forma correcta
+3, Hacer clic en el botón "Send"
+4, Confirmar que aparezca alerta  de envio correcto del mensaje</t>
+  </si>
+  <si>
+    <t>1, Hacer clic en el botón"Contact us"
+2, Dejar seleccionado el campo "-- Chose --"
+3, Hacer clic en el botón "Send"
+4, Confirmar que aparezca alerta con mensaje de error</t>
+  </si>
+  <si>
+    <t>Debe aparecer mensaje de error si no se llena el campo correo o sí se escribe mal.</t>
+  </si>
+  <si>
+    <t>1, Hacer clic en el boton "Contact us"
+2, Dejar el campo correo vacio
+3.Escribir el correo sin @ o sin .com</t>
+  </si>
+  <si>
+    <t>Debe aparecer mensaje de error si no se llena el campo de "mensaje"</t>
+  </si>
+  <si>
+    <t>1, Dejar vacio el campo Mensaje</t>
   </si>
 </sst>
 </file>
@@ -341,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -379,23 +411,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -420,6 +439,20 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1250,29 +1283,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="17" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
       <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="16"/>
+      <c r="A2" s="27"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1370,19 +1403,19 @@
         <v>16</v>
       </c>
       <c r="E4" s="4">
-        <f>COUNTIF(HU_002!H3:H50,"SI")</f>
+        <f>COUNTIF(HU_002!H3:H51,"SI")</f>
         <v>0</v>
       </c>
       <c r="F4" s="4">
-        <f>COUNTIF(HU_002!I3:I50,"SI")</f>
+        <f>COUNTIF(HU_002!I3:I51,"SI")</f>
         <v>0</v>
       </c>
       <c r="G4" s="4">
-        <f>COUNTA(HU_002!H3:H50)</f>
+        <f>COUNTA(HU_002!H3:H51)</f>
         <v>0</v>
       </c>
       <c r="H4" s="4">
-        <f>COUNTA(HU_002!J3:J50)</f>
+        <f>COUNTA(HU_002!J3:J51)</f>
         <v>0</v>
       </c>
       <c r="I4" s="4">
@@ -1390,19 +1423,19 @@
         <v>0</v>
       </c>
       <c r="J4" s="4">
-        <f>COUNTIF(HU_002!J3:J50,"EXITOSO")</f>
+        <f>COUNTIF(HU_002!J3:J51,"EXITOSO")</f>
         <v>0</v>
       </c>
       <c r="K4" s="4">
-        <f>COUNTIF(HU_002!J3:J50,"FALLIDO")</f>
+        <f>COUNTIF(HU_002!J3:J51,"FALLIDO")</f>
         <v>0</v>
       </c>
       <c r="L4" s="4">
-        <f>COUNTIF(HU_002!J3:J50,"N/A")</f>
+        <f>COUNTIF(HU_002!J3:J51,"N/A")</f>
         <v>0</v>
       </c>
       <c r="M4" s="4">
-        <f>SUM(HU_002!M3:M50)</f>
+        <f>SUM(HU_002!M3:M51)</f>
         <v>0</v>
       </c>
     </row>
@@ -1441,10 +1474,10 @@
   <dimension ref="A1:Y14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1459,46 +1492,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="12.75">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
     </row>
     <row r="2" spans="1:25" ht="12.75">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
       <c r="I2" s="1" t="s">
         <v>25</v>
       </c>
@@ -1519,22 +1552,22 @@
       <c r="B3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="19" t="s">
         <v>31</v>
       </c>
       <c r="I3" s="7"/>
@@ -1556,28 +1589,28 @@
       <c r="Y3" s="9"/>
     </row>
     <row r="4" spans="1:25" ht="60">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="19" t="s">
         <v>31</v>
       </c>
       <c r="I4" s="7"/>
@@ -1599,28 +1632,28 @@
       <c r="Y4" s="9"/>
     </row>
     <row r="5" spans="1:25" ht="63.75">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="19" t="s">
         <v>31</v>
       </c>
       <c r="I5" s="7"/>
@@ -1642,28 +1675,28 @@
       <c r="Y5" s="9"/>
     </row>
     <row r="6" spans="1:25" ht="76.5">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="H6" s="20" t="s">
         <v>31</v>
       </c>
       <c r="I6" s="6"/>
@@ -1672,28 +1705,28 @@
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:25" ht="114.75">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="20" t="s">
         <v>31</v>
       </c>
       <c r="I7" s="6"/>
@@ -1702,28 +1735,28 @@
       <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:25" ht="76.5">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="20" t="s">
         <v>31</v>
       </c>
       <c r="I8" s="6"/>
@@ -1732,28 +1765,28 @@
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:25" ht="30">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="20" t="s">
         <v>31</v>
       </c>
       <c r="I9" s="14"/>
@@ -1841,13 +1874,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z20"/>
+  <dimension ref="A1:Z21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1860,51 +1893,51 @@
     <col min="12" max="13" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:26" ht="12.75">
+      <c r="A1" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-    </row>
-    <row r="2" spans="1:26">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+    </row>
+    <row r="2" spans="1:26" ht="12.75">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
       <c r="J2" s="1" t="s">
         <v>25</v>
       </c>
@@ -1947,22 +1980,22 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="1:26" ht="60">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="19" t="s">
         <v>30</v>
       </c>
       <c r="G4" s="9"/>
@@ -1987,22 +2020,22 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="1:26" ht="45">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="19" t="s">
         <v>30</v>
       </c>
       <c r="G5" s="9"/>
@@ -2027,22 +2060,24 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="1:26" ht="60">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -2050,65 +2085,113 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="1:26" ht="12.75">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="7"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
+    <row r="7" spans="1:26" s="15" customFormat="1" ht="64.5">
+      <c r="A7" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
       <c r="K7" s="10"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" spans="1:26">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+    </row>
+    <row r="8" spans="1:26" ht="51">
+      <c r="A8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>39</v>
+      </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
+      <c r="L8" s="6"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="1:26">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="7"/>
+    <row r="9" spans="1:26" ht="45">
+      <c r="A9" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>39</v>
+      </c>
       <c r="G9" s="11"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="6"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
       <c r="M9" s="6"/>
     </row>
-    <row r="10" spans="1:26">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="7"/>
+    <row r="10" spans="1:26" ht="25.5">
+      <c r="A10" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="11"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
-      <c r="K10" s="10"/>
+      <c r="K10" s="12"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" ht="12.75">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="10"/>
@@ -2118,8 +2201,11 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="1:26">
+      <c r="K11" s="10"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="1:26" ht="12.75">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="10"/>
@@ -2129,11 +2215,8 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-    </row>
-    <row r="13" spans="1:26">
+    </row>
+    <row r="13" spans="1:26" ht="12.75">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="10"/>
@@ -2147,14 +2230,13 @@
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" ht="12.75">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="6"/>
+      <c r="E14" s="10"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="11"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
@@ -2162,54 +2244,58 @@
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" ht="12.75">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
       <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="1:26">
+      <c r="K15" s="10"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+    </row>
+    <row r="16" spans="1:26" ht="12.75">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="6"/>
+      <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="1:13" ht="12.75">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="K17" s="10"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+    </row>
+    <row r="18" spans="1:13" ht="12.75">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
+      <c r="E18" s="1"/>
       <c r="F18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" ht="12.75">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="10"/>
@@ -2218,16 +2304,13 @@
       <c r="F19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" ht="12.75">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="10"/>
-      <c r="D20" s="6"/>
+      <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="6"/>
       <c r="H20" s="6"/>
@@ -2236,6 +2319,20 @@
       <c r="K20" s="10"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
+    </row>
+    <row r="21" spans="1:13" ht="12.75">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2251,5 +2348,6 @@
     <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se agrega el reporte de pruebas, junto con reporte generado por selenium Junit y el diseño de pruebas en formato excel
</commit_message>
<xml_diff>
--- a/Diseño de pruebas.xlsx
+++ b/Diseño de pruebas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sofka\curso\6. Automatizacion\Reto1\AutomatizacionSelenium\RetoAutoSelenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7757298-10D4-4A13-9CAC-68A56F892E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CD2009-4412-4860-82C1-63432746DDA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consolidado" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="77">
   <si>
     <t>Módulo</t>
   </si>
@@ -286,6 +286,12 @@
   </si>
   <si>
     <t>1, Dejar vacio el campo Mensaje</t>
+  </si>
+  <si>
+    <t>EXITOSO</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -590,7 +596,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -664,10 +670,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1263,7 +1269,7 @@
   </sheetPr>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
@@ -1349,7 +1355,7 @@
       </c>
       <c r="B3" s="4">
         <f t="shared" ref="B3:B4" si="0">((H3*100)/G3)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -1368,15 +1374,15 @@
       </c>
       <c r="H3" s="1">
         <f>COUNTA(HU_001!I3:I50)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I3" s="4">
         <f t="shared" ref="I3:I4" si="1">G3-H3</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="J3" s="4">
         <f>COUNTIF(HU_001!I3:I50,"EXITOSO")</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K3" s="4">
         <f>COUNTIF(HU_001!I3:I50,"FALLIDO")</f>
@@ -1395,28 +1401,28 @@
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="4" t="e">
+      <c r="B4" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>100</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="4">
         <f>COUNTIF(HU_002!H3:H51,"SI")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F4" s="4">
         <f>COUNTIF(HU_002!I3:I51,"SI")</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G4" s="4">
         <f>COUNTA(HU_002!H3:H51)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H4" s="4">
         <f>COUNTA(HU_002!J3:J51)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I4" s="4">
         <f t="shared" si="1"/>
@@ -1424,7 +1430,7 @@
       </c>
       <c r="J4" s="4">
         <f>COUNTIF(HU_002!J3:J51,"EXITOSO")</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K4" s="4">
         <f>COUNTIF(HU_002!J3:J51,"FALLIDO")</f>
@@ -1570,7 +1576,9 @@
       <c r="H3" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="I3" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
@@ -1613,7 +1621,9 @@
       <c r="H4" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="I4" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
@@ -1656,7 +1666,9 @@
       <c r="H5" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="7"/>
+      <c r="I5" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
       <c r="L5" s="7"/>
@@ -1699,7 +1711,9 @@
       <c r="H6" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="6"/>
+      <c r="I6" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="J6" s="10"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
@@ -1729,7 +1743,9 @@
       <c r="H7" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="6"/>
+      <c r="I7" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="J7" s="10"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
@@ -1759,7 +1775,9 @@
       <c r="H8" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="6"/>
+      <c r="I8" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
       <c r="L8" s="6"/>
@@ -1789,7 +1807,9 @@
       <c r="H9" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="I9" s="14"/>
+      <c r="I9" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="J9" s="13"/>
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
@@ -1876,11 +1896,11 @@
   </sheetPr>
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1999,9 +2019,15 @@
         <v>30</v>
       </c>
       <c r="G4" s="9"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="H4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
       <c r="M4" s="7"/>
@@ -2039,9 +2065,15 @@
         <v>30</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="H5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
       <c r="M5" s="7"/>
@@ -2078,9 +2110,15 @@
       <c r="F6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
+      <c r="H6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="K6" s="10"/>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
@@ -2104,9 +2142,15 @@
       <c r="F7" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
+      <c r="H7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="K7" s="10"/>
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
@@ -2130,9 +2174,15 @@
       <c r="F8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
+      <c r="H8" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="K8" s="10"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
@@ -2157,9 +2207,15 @@
         <v>39</v>
       </c>
       <c r="G9" s="11"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
+      <c r="H9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
       <c r="M9" s="6"/>
@@ -2184,9 +2240,15 @@
         <v>39</v>
       </c>
       <c r="G10" s="11"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
+      <c r="H10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="K10" s="12"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>

</xml_diff>